<commit_message>
[feat] img buffer data crawling
</commit_message>
<xml_diff>
--- a/study/store/xlsx/result.xlsx
+++ b/study/store/xlsx/result.xlsx
@@ -1469,7 +1469,7 @@
         <v>9.51</v>
       </c>
       <c r="D2" t="str">
-        <v>https://movie-phinf.pstatic.net/20220516_144/1652665409592Chvey_JPEG/movie_image.jpg?type=m203_290_2</v>
+        <v>https://movie-phinf.pstatic.net/20220516_144/1652665409592Chvey_JPEG/movie_image.jpg</v>
       </c>
     </row>
     <row r="3">
@@ -1483,7 +1483,7 @@
         <v>8.73</v>
       </c>
       <c r="D3" t="str">
-        <v>https://movie-phinf.pstatic.net/20191024_143/1571893663418kwLN7_JPEG/movie_image.jpg?type=m203_290_2</v>
+        <v>https://movie-phinf.pstatic.net/20191024_143/1571893663418kwLN7_JPEG/movie_image.jpg</v>
       </c>
     </row>
     <row r="4">
@@ -1497,7 +1497,7 @@
         <v>8.65</v>
       </c>
       <c r="D4" t="str">
-        <v>https://movie-phinf.pstatic.net/20111224_165/13246577572754h14b_JPEG/movie_image.jpg?type=m203_290_2</v>
+        <v>https://movie-phinf.pstatic.net/20111224_165/13246577572754h14b_JPEG/movie_image.jpg</v>
       </c>
     </row>
     <row r="5">
@@ -1511,7 +1511,7 @@
         <v>8.55</v>
       </c>
       <c r="D5" t="str">
-        <v>https://movie-phinf.pstatic.net/20130204_279/1359954210596SuaVm_JPEG/movie_image.jpg?type=m203_290_2</v>
+        <v>https://movie-phinf.pstatic.net/20130204_279/1359954210596SuaVm_JPEG/movie_image.jpg</v>
       </c>
     </row>
     <row r="6">
@@ -1525,7 +1525,7 @@
         <v>8.40</v>
       </c>
       <c r="D6" t="str">
-        <v>https://movie-phinf.pstatic.net/20111223_87/13245909373833oAeh_JPEG/movie_image.jpg?type=m203_290_2</v>
+        <v>https://movie-phinf.pstatic.net/20111223_87/13245909373833oAeh_JPEG/movie_image.jpg</v>
       </c>
     </row>
   </sheetData>

</xml_diff>